<commit_message>
modified excel files where there were wrong values in the lookup table
</commit_message>
<xml_diff>
--- a/python-server/server-master/Python/dataset/dataset_for_server.xlsx
+++ b/python-server/server-master/Python/dataset/dataset_for_server.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\Iva\PoliTO\TESI\Dyscalculia\python-server\server-master\Python\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaia1\Documents\0_Documenti\Dyscalculia\GitHub\python-server\server-master\Python\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5512C197-8694-4569-A197-86452739A64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E16B46-4D5C-488B-BD54-57060650066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{C98A85C0-7722-4B44-83C8-0DB810962166}"/>
+    <workbookView xWindow="-16110" yWindow="-760" windowWidth="16220" windowHeight="11500" xr2:uid="{C98A85C0-7722-4B44-83C8-0DB810962166}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +126,9 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{12CC16F4-4715-40D5-977A-649635F494C8}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,18 +439,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82F7068-7C51-4FA6-BB9C-D515079B8E2A}">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C240" sqref="C240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="18.28515625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="18.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>21</v>
       </c>
@@ -470,7 +472,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>21</v>
       </c>
@@ -481,7 +483,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -492,7 +494,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>27</v>
       </c>
@@ -503,7 +505,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>37</v>
       </c>
@@ -514,7 +516,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>37</v>
       </c>
@@ -525,7 +527,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45</v>
       </c>
@@ -536,7 +538,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>48</v>
       </c>
@@ -547,7 +549,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>61</v>
       </c>
@@ -558,7 +560,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -569,7 +571,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -580,7 +582,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>69</v>
       </c>
@@ -591,7 +593,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>89</v>
       </c>
@@ -602,7 +604,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>97</v>
       </c>
@@ -613,7 +615,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>101</v>
       </c>
@@ -624,7 +626,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>112</v>
       </c>
@@ -635,7 +637,7 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -646,7 +648,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -657,7 +659,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>21</v>
       </c>
@@ -668,7 +670,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -679,7 +681,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>25</v>
       </c>
@@ -690,7 +692,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>29</v>
       </c>
@@ -701,7 +703,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>37</v>
       </c>
@@ -712,7 +714,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>37</v>
       </c>
@@ -723,7 +725,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45</v>
       </c>
@@ -734,7 +736,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45</v>
       </c>
@@ -745,7 +747,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>57</v>
       </c>
@@ -756,7 +758,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>61</v>
       </c>
@@ -767,7 +769,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>69</v>
       </c>
@@ -778,7 +780,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>69</v>
       </c>
@@ -789,7 +791,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>81</v>
       </c>
@@ -800,7 +802,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>89</v>
       </c>
@@ -811,7 +813,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>9</v>
       </c>
@@ -822,7 +824,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>9</v>
       </c>
@@ -833,7 +835,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>13</v>
       </c>
@@ -844,7 +846,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>21</v>
       </c>
@@ -855,7 +857,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>21</v>
       </c>
@@ -866,7 +868,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>21</v>
       </c>
@@ -877,7 +879,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>25</v>
       </c>
@@ -888,7 +890,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>29</v>
       </c>
@@ -899,7 +901,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>37</v>
       </c>
@@ -910,7 +912,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>37</v>
       </c>
@@ -921,7 +923,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -932,7 +934,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -943,7 +945,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -954,7 +956,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>61</v>
       </c>
@@ -965,7 +967,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>69</v>
       </c>
@@ -976,7 +978,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>69</v>
       </c>
@@ -987,7 +989,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>9</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>9</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>9</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>13</v>
       </c>
@@ -1031,9 +1033,9 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B54" s="1">
         <v>11736.11</v>
@@ -1042,7 +1044,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>21</v>
       </c>
@@ -1053,7 +1055,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>21</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>21</v>
       </c>
@@ -1075,9 +1077,9 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" s="1">
         <v>20069.439999999999</v>
@@ -1086,7 +1088,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>37</v>
       </c>
@@ -1097,7 +1099,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>37</v>
       </c>
@@ -1108,7 +1110,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>37</v>
       </c>
@@ -1119,7 +1121,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>45</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>49</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>57</v>
       </c>
@@ -1163,7 +1165,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>9</v>
       </c>
@@ -1174,7 +1176,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>9</v>
       </c>
@@ -1185,7 +1187,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>9</v>
       </c>
@@ -1196,7 +1198,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>9</v>
       </c>
@@ -1207,9 +1209,9 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B70" s="1">
         <v>11736.11</v>
@@ -1218,7 +1220,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>13</v>
       </c>
@@ -1229,7 +1231,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>21</v>
       </c>
@@ -1240,7 +1242,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>21</v>
       </c>
@@ -1251,7 +1253,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>21</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>25</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>29</v>
       </c>
@@ -1284,7 +1286,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>29</v>
       </c>
@@ -1295,7 +1297,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>37</v>
       </c>
@@ -1306,9 +1308,9 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B79" s="1">
         <v>33611.11</v>
@@ -1317,7 +1319,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45</v>
       </c>
@@ -1328,7 +1330,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>45</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>62.33</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>5</v>
       </c>
@@ -1347,10 +1349,10 @@
         <v>5625</v>
       </c>
       <c r="C82" s="4">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>9</v>
       </c>
@@ -1358,10 +1360,10 @@
         <v>6944.44</v>
       </c>
       <c r="C83" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>9</v>
       </c>
@@ -1369,10 +1371,10 @@
         <v>8402.7800000000007</v>
       </c>
       <c r="C84" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>9</v>
       </c>
@@ -1380,10 +1382,10 @@
         <v>10000</v>
       </c>
       <c r="C85" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>9</v>
       </c>
@@ -1391,10 +1393,10 @@
         <v>11736.11</v>
       </c>
       <c r="C86" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>13</v>
       </c>
@@ -1402,10 +1404,10 @@
         <v>13611.11</v>
       </c>
       <c r="C87" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>21</v>
       </c>
@@ -1413,10 +1415,10 @@
         <v>15625</v>
       </c>
       <c r="C88" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>21</v>
       </c>
@@ -1424,10 +1426,10 @@
         <v>17777.78</v>
       </c>
       <c r="C89" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>21</v>
       </c>
@@ -1435,10 +1437,10 @@
         <v>20069.439999999999</v>
       </c>
       <c r="C90" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>21</v>
       </c>
@@ -1446,32 +1448,32 @@
         <v>22500</v>
       </c>
       <c r="C91" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B92" s="1">
         <v>25069.439999999999</v>
       </c>
       <c r="C92" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B93" s="1">
         <v>27777.78</v>
       </c>
       <c r="C93" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>29</v>
       </c>
@@ -1479,10 +1481,10 @@
         <v>30625</v>
       </c>
       <c r="C94" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>37</v>
       </c>
@@ -1490,10 +1492,10 @@
         <v>33611.11</v>
       </c>
       <c r="C95" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>37</v>
       </c>
@@ -1501,10 +1503,10 @@
         <v>36736.11</v>
       </c>
       <c r="C96" s="5">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>37</v>
       </c>
@@ -1512,10 +1514,10 @@
         <v>40000</v>
       </c>
       <c r="C97" s="3">
-        <v>79.95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>5</v>
       </c>
@@ -1526,9 +1528,9 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B99" s="1">
         <v>6944.44</v>
@@ -1537,7 +1539,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>9</v>
       </c>
@@ -1548,7 +1550,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>9</v>
       </c>
@@ -1559,7 +1561,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>9</v>
       </c>
@@ -1570,9 +1572,9 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B103" s="1">
         <v>13611.11</v>
@@ -1581,7 +1583,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>13</v>
       </c>
@@ -1592,7 +1594,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>13</v>
       </c>
@@ -1603,7 +1605,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>21</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>21</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>21</v>
       </c>
@@ -1636,9 +1638,9 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B109" s="1">
         <v>27777.78</v>
@@ -1647,7 +1649,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>25</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>25</v>
       </c>
@@ -1669,7 +1671,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>29</v>
       </c>
@@ -1680,7 +1682,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>37</v>
       </c>
@@ -1691,7 +1693,7 @@
         <v>93.11</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>1</v>
       </c>
@@ -1702,7 +1704,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>9</v>
       </c>
@@ -1713,7 +1715,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>9</v>
       </c>
@@ -1724,7 +1726,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>9</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>9</v>
       </c>
@@ -1746,7 +1748,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>9</v>
       </c>
@@ -1757,9 +1759,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B120" s="1">
         <v>15625</v>
@@ -1768,7 +1770,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>13</v>
       </c>
@@ -1779,9 +1781,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B122" s="1">
         <v>20069.439999999999</v>
@@ -1790,7 +1792,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>21</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>21</v>
       </c>
@@ -1812,7 +1814,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>21</v>
       </c>
@@ -1823,9 +1825,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B126" s="1">
         <v>30625</v>
@@ -1834,9 +1836,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B127" s="1">
         <v>33611.11</v>
@@ -1845,9 +1847,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B128" s="1">
         <v>36736.11</v>
@@ -1856,9 +1858,9 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B129" s="3">
         <v>40000</v>
@@ -1867,7 +1869,7 @@
         <v>110.8</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>1</v>
       </c>
@@ -1878,7 +1880,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>5</v>
       </c>
@@ -1889,7 +1891,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>5</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>9</v>
       </c>
@@ -1911,7 +1913,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>9</v>
       </c>
@@ -1922,7 +1924,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>9</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>9</v>
       </c>
@@ -1944,7 +1946,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>9</v>
       </c>
@@ -1955,7 +1957,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>13</v>
       </c>
@@ -1966,9 +1968,9 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B139" s="1">
         <v>22500</v>
@@ -1977,7 +1979,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>21</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>21</v>
       </c>
@@ -1999,7 +2001,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>21</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>21</v>
       </c>
@@ -2021,7 +2023,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>21</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>25</v>
       </c>
@@ -2043,7 +2045,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>1</v>
       </c>
@@ -2054,7 +2056,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>5</v>
       </c>
@@ -2065,7 +2067,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>5</v>
       </c>
@@ -2076,7 +2078,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>5</v>
       </c>
@@ -2087,7 +2089,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>9</v>
       </c>
@@ -2098,7 +2100,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>9</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>9</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>9</v>
       </c>
@@ -2131,7 +2133,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>9</v>
       </c>
@@ -2142,7 +2144,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>9</v>
       </c>
@@ -2153,7 +2155,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>13</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>13</v>
       </c>
@@ -2175,9 +2177,9 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B158" s="1">
         <v>30625</v>
@@ -2186,7 +2188,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>21</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>21</v>
       </c>
@@ -2208,7 +2210,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>21</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>150.82</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>1</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>5</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>5</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>5</v>
       </c>
@@ -2263,9 +2265,9 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B166" s="1">
         <v>11736.11</v>
@@ -2274,7 +2276,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>9</v>
       </c>
@@ -2285,7 +2287,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>9</v>
       </c>
@@ -2296,9 +2298,9 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B169" s="1">
         <v>17777.78</v>
@@ -2307,7 +2309,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>9</v>
       </c>
@@ -2318,7 +2320,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>9</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>9</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>13</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>13</v>
       </c>
@@ -2362,7 +2364,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>21</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>21</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="3">
         <v>21</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>173.13</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>1</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>1</v>
       </c>
@@ -2417,7 +2419,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>5</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>5</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>5</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>5</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>9</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>9</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>9</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>9</v>
       </c>
@@ -2505,7 +2507,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>9</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>9</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>13</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>13</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>21</v>
       </c>
@@ -2560,7 +2562,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="3">
         <v>21</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>196.98</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>1</v>
       </c>
@@ -2582,7 +2584,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>1</v>
       </c>
@@ -2593,7 +2595,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>1</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>5</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>5</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>5</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>5</v>
       </c>
@@ -2648,7 +2650,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>9</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>9</v>
       </c>
@@ -2670,7 +2672,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>9</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>9</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>9</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>9</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>13</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>13</v>
       </c>
@@ -2736,7 +2738,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="3">
         <v>13</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>222.38</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>1</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>1</v>
       </c>
@@ -2769,7 +2771,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>1</v>
       </c>
@@ -2780,7 +2782,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>1</v>
       </c>
@@ -2791,7 +2793,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>5</v>
       </c>
@@ -2802,7 +2804,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>5</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>5</v>
       </c>
@@ -2824,7 +2826,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>9</v>
       </c>
@@ -2835,7 +2837,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>9</v>
       </c>
@@ -2846,7 +2848,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>9</v>
       </c>
@@ -2857,7 +2859,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>9</v>
       </c>
@@ -2868,7 +2870,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>9</v>
       </c>
@@ -2879,7 +2881,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>9</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>9</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>13</v>
       </c>
@@ -2912,7 +2914,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A225" s="3">
         <v>13</v>
       </c>
@@ -2923,7 +2925,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>1</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>1</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>1</v>
       </c>
@@ -2956,7 +2958,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>1</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>5</v>
       </c>
@@ -2978,7 +2980,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>5</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>5</v>
       </c>
@@ -3000,7 +3002,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>5</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>9</v>
       </c>
@@ -3022,7 +3024,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>9</v>
       </c>
@@ -3033,7 +3035,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>9</v>
       </c>
@@ -3044,7 +3046,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>9</v>
       </c>
@@ -3055,7 +3057,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>9</v>
       </c>
@@ -3066,7 +3068,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>9</v>
       </c>
@@ -3077,9 +3079,9 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B240" s="1">
         <v>36736.11</v>
@@ -3088,7 +3090,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A241" s="3">
         <v>13</v>
       </c>
@@ -3099,7 +3101,7 @@
         <v>277.77999999999997</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>1</v>
       </c>
@@ -3110,7 +3112,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>1</v>
       </c>
@@ -3121,7 +3123,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>1</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>1</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>1</v>
       </c>
@@ -3154,7 +3156,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>5</v>
       </c>
@@ -3165,7 +3167,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>5</v>
       </c>
@@ -3176,7 +3178,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>5</v>
       </c>
@@ -3187,7 +3189,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>5</v>
       </c>
@@ -3198,7 +3200,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>9</v>
       </c>
@@ -3209,7 +3211,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>9</v>
       </c>
@@ -3220,7 +3222,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>9</v>
       </c>
@@ -3231,7 +3233,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>9</v>
       </c>
@@ -3242,7 +3244,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>9</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>9</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>307.79000000000002</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>9</v>
       </c>

</xml_diff>